<commit_message>
adding figures to markdown
</commit_message>
<xml_diff>
--- a/FieldMuseum.xlsx
+++ b/FieldMuseum.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Chicago Park District property tax remittances</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>net_assets_ending</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -715,7 +721,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1848,6 +1854,38 @@
         <v>339201536</v>
       </c>
     </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2005</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2006</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2007</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2008</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2009</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2010</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2011</v>
+      </c>
+    </row>
     <row r="37" spans="1:10">
       <c r="H37" t="s">
         <v>37</v>

</xml_diff>